<commit_message>
7- Added New Fn
</commit_message>
<xml_diff>
--- a/Resources/7-CustomClubOrderEntry.xlsx
+++ b/Resources/7-CustomClubOrderEntry.xlsx
@@ -627,7 +627,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -663,7 +663,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
7-ConfigI1 and Updated Spread sheet
</commit_message>
<xml_diff>
--- a/Resources/7-CustomClubOrderEntry.xlsx
+++ b/Resources/7-CustomClubOrderEntry.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>CustomerNumber</t>
   </si>
@@ -86,9 +86,6 @@
     <t>CUSTOM  CLUB 5</t>
   </si>
   <si>
-    <t>CUSTOM  CLUB 6</t>
-  </si>
-  <si>
     <t>CUSTOM  CLUB 7</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>DAVE</t>
   </si>
   <si>
-    <t>STEVE</t>
-  </si>
-  <si>
     <t>JIM</t>
   </si>
   <si>
@@ -134,9 +128,6 @@
     <t>F03</t>
   </si>
   <si>
-    <t>F04</t>
-  </si>
-  <si>
     <t>632C</t>
   </si>
   <si>
@@ -162,9 +153,6 @@
   </si>
   <si>
     <t>ConfigD5</t>
-  </si>
-  <si>
-    <t>ConfigD6</t>
   </si>
   <si>
     <t>ConfigI1</t>
@@ -562,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +576,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
@@ -603,7 +591,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>10</v>
@@ -624,7 +612,7 @@
         <v>4</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -632,13 +620,13 @@
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>5</v>
@@ -648,7 +636,7 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -660,7 +648,7 @@
         <v>5</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -668,23 +656,23 @@
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -696,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -704,23 +692,23 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -732,7 +720,7 @@
         <v>5</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -740,23 +728,23 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -768,7 +756,7 @@
         <v>5</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -776,13 +764,13 @@
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>5</v>
@@ -792,7 +780,7 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
@@ -804,7 +792,7 @@
         <v>5</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -812,23 +800,23 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
@@ -837,24 +825,24 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>5</v>
@@ -864,7 +852,7 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="3">
         <v>1</v>
@@ -876,21 +864,21 @@
         <v>2</v>
       </c>
       <c r="N8" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>5</v>
@@ -900,7 +888,7 @@
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
@@ -909,47 +897,27 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="3">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="3">
-        <v>4</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -1094,22 +1062,6 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update data files for #1 and #7
</commit_message>
<xml_diff>
--- a/Resources/7-CustomClubOrderEntry.xlsx
+++ b/Resources/7-CustomClubOrderEntry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="28830" windowHeight="6405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -15,11 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
   <si>
     <t>CustomerNumber</t>
   </si>
   <si>
+    <t>US00028338</t>
+  </si>
+  <si>
     <t>FXG</t>
   </si>
   <si>
@@ -59,15 +62,108 @@
     <t>US00025028</t>
   </si>
   <si>
+    <t>US00025065</t>
+  </si>
+  <si>
+    <t>US00064622</t>
+  </si>
+  <si>
+    <t>US00002181</t>
+  </si>
+  <si>
+    <t>CUSTOM  CLUB 1</t>
+  </si>
+  <si>
+    <t>CUSTOM  CLUB 2</t>
+  </si>
+  <si>
+    <t>CUSTOM  CLUB 3</t>
+  </si>
+  <si>
+    <t>CUSTOM  CLUB 4</t>
+  </si>
+  <si>
+    <t>CUSTOM  CLUB 5</t>
+  </si>
+  <si>
+    <t>CUSTOM  CLUB 7</t>
+  </si>
+  <si>
+    <t>CUSTOM  CLUB 8</t>
+  </si>
+  <si>
+    <t>CUSTOM  CLUB 9</t>
+  </si>
+  <si>
     <t>JOHN</t>
   </si>
   <si>
+    <t>JOE</t>
+  </si>
+  <si>
+    <t>BILL</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>DAVE</t>
+  </si>
+  <si>
+    <t>JIM</t>
+  </si>
+  <si>
+    <t>STAN</t>
+  </si>
+  <si>
+    <t>CHRIS</t>
+  </si>
+  <si>
+    <t>F00</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>F03</t>
+  </si>
+  <si>
     <t>632C</t>
   </si>
   <si>
+    <t>529C</t>
+  </si>
+  <si>
+    <t>832C</t>
+  </si>
+  <si>
+    <t>733C</t>
+  </si>
+  <si>
     <t>ConfigD1</t>
   </si>
   <si>
+    <t>ConfigD2</t>
+  </si>
+  <si>
+    <t>ConfigD3</t>
+  </si>
+  <si>
+    <t>ConfigD4</t>
+  </si>
+  <si>
+    <t>ConfigD5</t>
+  </si>
+  <si>
+    <t>ConfigI1</t>
+  </si>
+  <si>
+    <t>Config W1</t>
+  </si>
+  <si>
+    <t>ConfigP1</t>
+  </si>
+  <si>
     <t>Configuration</t>
   </si>
   <si>
@@ -78,9 +174,6 @@
   </si>
   <si>
     <t>WHNumber</t>
-  </si>
-  <si>
-    <t>CLUB-010-COM</t>
   </si>
 </sst>
 </file>
@@ -457,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,67 +576,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -555,136 +648,276 @@
         <v>5</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="3">
+        <v>5</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="3">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="3">
+        <v>5</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="B5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3">
+        <v>5</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3">
+        <v>5</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="3">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="3">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="3">
+        <v>4</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -717,6 +950,134 @@
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -734,172 +1095,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Unknown Document Type" ma:contentTypeID="0x010104" ma:contentTypeVersion="0" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="05d83ceaa0bbd2e3bc716e6e66bd857a">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3d69fe45253d5ff147bb69036b756a7">
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all/>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type" ma:readOnly="true"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="3" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B04528D7-AFCA-46C1-B69E-C17D778EE671}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B81A40B-79C7-4BD0-AB25-EB4A4CE7B262}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2535B56B-199C-4FF1-B352-25B534CE0D60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>